<commit_message>
correção de alguns arquivos
</commit_message>
<xml_diff>
--- a/Tratamento com Python/Etapa 1/Comparação dos campos de cada tabela.xlsx
+++ b/Tratamento com Python/Etapa 1/Comparação dos campos de cada tabela.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Meu Drive\Unversidade\Iniciacão Cientifica\Tratamento em Python\Etapa 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\GenderViolence-DataVis\Tratamento com Python\Etapa 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5412C8AB-397E-4286-A13B-84F7F1DCB63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100C99F7-A558-4744-B65D-996A98C0C4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="157">
   <si>
     <t>Data de cadastro</t>
   </si>
@@ -88,13 +88,13 @@
     <t>Filhos violência</t>
   </si>
   <si>
-    <t>Violação</t>
+    <t>Violações</t>
   </si>
   <si>
     <t>UF</t>
   </si>
   <si>
-    <t>Munícipio</t>
+    <t>Município</t>
   </si>
   <si>
     <t>Residência</t>
@@ -148,7 +148,7 @@
     <t>Suspeito cod municipio</t>
   </si>
   <si>
-    <t>sl suspeito municipio</t>
+    <t>Município do suspeito</t>
   </si>
   <si>
     <t>UF do suspeito</t>
@@ -175,21 +175,12 @@
     <t>Suspeito pj qualificação jurídica</t>
   </si>
   <si>
-    <t>Violações</t>
-  </si>
-  <si>
     <t>2020-1</t>
   </si>
   <si>
-    <t>País de orígem da vítima</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
-    <t>Município</t>
-  </si>
-  <si>
     <t>Faixa de renda da vítima</t>
   </si>
   <si>
@@ -211,7 +202,7 @@
     <t>País do suspeito</t>
   </si>
   <si>
-    <t>País de orígem do suspeito</t>
+    <t>Nacionalidade do suspeito</t>
   </si>
   <si>
     <t>Etnia da vítima</t>
@@ -275,9 +266,6 @@
   </si>
   <si>
     <t>Natureza Jurídica do Suspeito</t>
-  </si>
-  <si>
-    <t>Suspeito nacionalidade</t>
   </si>
   <si>
     <t>sl suspeito naturalidade</t>
@@ -509,7 +497,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,12 +521,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -649,19 +631,21 @@
     <xf numFmtId="3" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,81 +954,81 @@
   <dimension ref="A1:BK26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.21875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="31" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="29" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="26" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="46.88671875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="35.88671875" customWidth="1"/>
-    <col min="63" max="63" width="22" customWidth="1"/>
+    <col min="44" max="44" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:63" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2014</v>
       </c>
@@ -1127,7 +1111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2015</v>
       </c>
@@ -1210,7 +1194,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2016</v>
       </c>
@@ -1293,7 +1277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
@@ -1376,7 +1360,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -1459,7 +1443,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1566,10 +1550,10 @@
         <v>50</v>
       </c>
       <c r="AJ7" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2019</v>
       </c>
@@ -1676,12 +1660,12 @@
         <v>50</v>
       </c>
       <c r="AJ8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -1696,16 +1680,16 @@
         <v>28</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="G9" t="s">
         <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="J9" t="s">
         <v>33</v>
@@ -1723,13 +1707,13 @@
         <v>9</v>
       </c>
       <c r="O9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="P9" t="s">
         <v>7</v>
       </c>
       <c r="Q9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="R9" t="s">
         <v>15</v>
@@ -1741,54 +1725,54 @@
         <v>18</v>
       </c>
       <c r="U9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="V9" t="s">
         <v>16</v>
       </c>
       <c r="W9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="X9" t="s">
         <v>14</v>
       </c>
       <c r="Y9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB9" t="s">
         <v>60</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AC9" t="s">
         <v>61</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AD9" t="s">
         <v>62</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AE9" t="s">
         <v>63</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AF9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG9" t="s">
         <v>64</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AH9" t="s">
         <v>65</v>
       </c>
-      <c r="AE9" t="s">
+    </row>
+    <row r="10" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AF9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG9" t="s">
+      <c r="B10" t="s">
         <v>67</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" t="s">
-        <v>70</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -1797,7 +1781,7 @@
         <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
@@ -1806,34 +1790,34 @@
         <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
         <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K10" t="s">
         <v>10</v>
       </c>
       <c r="L10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N10" t="s">
         <v>29</v>
       </c>
       <c r="O10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P10" t="s">
         <v>14</v>
       </c>
       <c r="Q10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R10" t="s">
         <v>6</v>
@@ -1845,31 +1829,31 @@
         <v>8</v>
       </c>
       <c r="U10" t="s">
+        <v>72</v>
+      </c>
+      <c r="V10" t="s">
+        <v>73</v>
+      </c>
+      <c r="W10" t="s">
+        <v>74</v>
+      </c>
+      <c r="X10" t="s">
         <v>75</v>
       </c>
-      <c r="V10" t="s">
+      <c r="Y10" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z10" t="s">
         <v>76</v>
       </c>
-      <c r="W10" t="s">
+      <c r="AA10" t="s">
         <v>77</v>
       </c>
-      <c r="X10" t="s">
+      <c r="AB10" t="s">
         <v>78</v>
       </c>
-      <c r="Y10" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>81</v>
-      </c>
       <c r="AC10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AD10" t="s">
         <v>37</v>
@@ -1878,25 +1862,25 @@
         <v>36</v>
       </c>
       <c r="AF10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG10" t="s">
         <v>9</v>
       </c>
       <c r="AH10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI10" t="s">
         <v>7</v>
       </c>
       <c r="AJ10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AK10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AL10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AM10" t="s">
         <v>15</v>
@@ -1908,31 +1892,31 @@
         <v>17</v>
       </c>
       <c r="AP10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU10" t="s">
         <v>85</v>
       </c>
-      <c r="AQ10" t="s">
+      <c r="AV10" t="s">
         <v>86</v>
       </c>
-      <c r="AR10" t="s">
+      <c r="AW10" t="s">
         <v>87</v>
       </c>
-      <c r="AS10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT10" t="s">
+      <c r="AX10" t="s">
         <v>59</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV10" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX10" t="s">
-        <v>62</v>
       </c>
       <c r="AY10" t="s">
         <v>43</v>
@@ -1941,45 +1925,45 @@
         <v>42</v>
       </c>
       <c r="BA10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="BB10" t="s">
         <v>18</v>
       </c>
       <c r="BC10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="BD10" t="s">
         <v>16</v>
       </c>
       <c r="BE10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="BF10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="BG10" t="s">
+        <v>90</v>
+      </c>
+      <c r="BH10" t="s">
+        <v>91</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="BH10" t="s">
-        <v>95</v>
-      </c>
-      <c r="BI10" t="s">
-        <v>96</v>
-      </c>
-      <c r="BJ10" t="s">
-        <v>97</v>
-      </c>
-      <c r="BK10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -1988,7 +1972,7 @@
         <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
@@ -1997,34 +1981,34 @@
         <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I11" t="s">
         <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K11" t="s">
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N11" t="s">
         <v>29</v>
       </c>
       <c r="O11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P11" t="s">
         <v>14</v>
       </c>
       <c r="Q11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R11" t="s">
         <v>6</v>
@@ -2036,31 +2020,31 @@
         <v>8</v>
       </c>
       <c r="U11" t="s">
+        <v>72</v>
+      </c>
+      <c r="V11" t="s">
+        <v>73</v>
+      </c>
+      <c r="W11" t="s">
+        <v>74</v>
+      </c>
+      <c r="X11" t="s">
         <v>75</v>
       </c>
-      <c r="V11" t="s">
+      <c r="Y11" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z11" t="s">
         <v>76</v>
       </c>
-      <c r="W11" t="s">
+      <c r="AA11" t="s">
         <v>77</v>
       </c>
-      <c r="X11" t="s">
+      <c r="AB11" t="s">
         <v>78</v>
       </c>
-      <c r="Y11" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>81</v>
-      </c>
       <c r="AC11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AD11" t="s">
         <v>37</v>
@@ -2069,25 +2053,25 @@
         <v>36</v>
       </c>
       <c r="AF11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG11" t="s">
         <v>9</v>
       </c>
       <c r="AH11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI11" t="s">
         <v>7</v>
       </c>
       <c r="AJ11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AK11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AL11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AM11" t="s">
         <v>15</v>
@@ -2099,31 +2083,31 @@
         <v>17</v>
       </c>
       <c r="AP11" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU11" t="s">
         <v>85</v>
       </c>
-      <c r="AQ11" t="s">
+      <c r="AV11" t="s">
         <v>86</v>
       </c>
-      <c r="AR11" t="s">
+      <c r="AW11" t="s">
         <v>87</v>
       </c>
-      <c r="AS11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT11" t="s">
+      <c r="AX11" t="s">
         <v>59</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX11" t="s">
-        <v>62</v>
       </c>
       <c r="AY11" t="s">
         <v>43</v>
@@ -2132,45 +2116,45 @@
         <v>42</v>
       </c>
       <c r="BA11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="BB11" t="s">
         <v>18</v>
       </c>
       <c r="BC11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="BD11" t="s">
         <v>16</v>
       </c>
       <c r="BE11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="BF11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="BG11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="BH11" t="s">
+        <v>91</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ11" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="BI11" t="s">
-        <v>96</v>
-      </c>
-      <c r="BJ11" t="s">
-        <v>97</v>
-      </c>
-      <c r="BK11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -2179,7 +2163,7 @@
         <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
@@ -2188,34 +2172,34 @@
         <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I12" t="s">
         <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K12" t="s">
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N12" t="s">
         <v>29</v>
       </c>
       <c r="O12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P12" t="s">
         <v>14</v>
       </c>
       <c r="Q12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R12" t="s">
         <v>6</v>
@@ -2227,31 +2211,31 @@
         <v>8</v>
       </c>
       <c r="U12" t="s">
+        <v>72</v>
+      </c>
+      <c r="V12" t="s">
+        <v>73</v>
+      </c>
+      <c r="W12" t="s">
+        <v>74</v>
+      </c>
+      <c r="X12" t="s">
         <v>75</v>
       </c>
-      <c r="V12" t="s">
+      <c r="Y12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z12" t="s">
         <v>76</v>
       </c>
-      <c r="W12" t="s">
+      <c r="AA12" t="s">
         <v>77</v>
       </c>
-      <c r="X12" t="s">
+      <c r="AB12" t="s">
         <v>78</v>
       </c>
-      <c r="Y12" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>81</v>
-      </c>
       <c r="AC12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AD12" t="s">
         <v>37</v>
@@ -2260,25 +2244,25 @@
         <v>36</v>
       </c>
       <c r="AF12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG12" t="s">
         <v>9</v>
       </c>
       <c r="AH12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI12" t="s">
         <v>7</v>
       </c>
       <c r="AJ12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AK12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AL12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AM12" t="s">
         <v>15</v>
@@ -2290,31 +2274,31 @@
         <v>17</v>
       </c>
       <c r="AP12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU12" t="s">
         <v>85</v>
       </c>
-      <c r="AQ12" t="s">
+      <c r="AV12" t="s">
         <v>86</v>
       </c>
-      <c r="AR12" t="s">
+      <c r="AW12" t="s">
         <v>87</v>
       </c>
-      <c r="AS12" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT12" t="s">
+      <c r="AX12" t="s">
         <v>59</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV12" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX12" t="s">
-        <v>62</v>
       </c>
       <c r="AY12" t="s">
         <v>43</v>
@@ -2323,45 +2307,45 @@
         <v>42</v>
       </c>
       <c r="BA12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="BB12" t="s">
         <v>18</v>
       </c>
       <c r="BC12" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="BD12" t="s">
         <v>16</v>
       </c>
       <c r="BE12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="BF12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="BG12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="BH12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="BI12" t="s">
+        <v>92</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="BJ12" t="s">
-        <v>97</v>
-      </c>
-      <c r="BK12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
@@ -2370,7 +2354,7 @@
         <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
         <v>3</v>
@@ -2379,34 +2363,34 @@
         <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I13" t="s">
         <v>23</v>
       </c>
       <c r="J13" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K13" t="s">
         <v>10</v>
       </c>
       <c r="L13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N13" t="s">
         <v>29</v>
       </c>
       <c r="O13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P13" t="s">
         <v>14</v>
       </c>
       <c r="Q13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R13" t="s">
         <v>6</v>
@@ -2418,31 +2402,31 @@
         <v>8</v>
       </c>
       <c r="U13" t="s">
+        <v>72</v>
+      </c>
+      <c r="V13" t="s">
+        <v>73</v>
+      </c>
+      <c r="W13" t="s">
+        <v>74</v>
+      </c>
+      <c r="X13" t="s">
         <v>75</v>
       </c>
-      <c r="V13" t="s">
+      <c r="Y13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z13" t="s">
         <v>76</v>
       </c>
-      <c r="W13" t="s">
+      <c r="AA13" t="s">
         <v>77</v>
       </c>
-      <c r="X13" t="s">
+      <c r="AB13" t="s">
         <v>78</v>
       </c>
-      <c r="Y13" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>81</v>
-      </c>
       <c r="AC13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AD13" t="s">
         <v>37</v>
@@ -2451,25 +2435,25 @@
         <v>36</v>
       </c>
       <c r="AF13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG13" t="s">
         <v>9</v>
       </c>
       <c r="AH13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI13" t="s">
         <v>7</v>
       </c>
       <c r="AJ13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AK13" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AL13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AM13" t="s">
         <v>15</v>
@@ -2481,31 +2465,31 @@
         <v>17</v>
       </c>
       <c r="AP13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU13" t="s">
         <v>85</v>
       </c>
-      <c r="AQ13" t="s">
+      <c r="AV13" t="s">
         <v>86</v>
       </c>
-      <c r="AR13" t="s">
+      <c r="AW13" t="s">
         <v>87</v>
       </c>
-      <c r="AS13" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT13" t="s">
+      <c r="AX13" t="s">
         <v>59</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV13" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX13" t="s">
-        <v>62</v>
       </c>
       <c r="AY13" t="s">
         <v>43</v>
@@ -2514,45 +2498,45 @@
         <v>42</v>
       </c>
       <c r="BA13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="BB13" t="s">
         <v>18</v>
       </c>
       <c r="BC13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="BD13" t="s">
         <v>16</v>
       </c>
       <c r="BE13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="BF13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="BG13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="BH13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="BI13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="BJ13" t="s">
+        <v>93</v>
+      </c>
+      <c r="BK13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="BK13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
@@ -2561,7 +2545,7 @@
         <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
         <v>3</v>
@@ -2570,34 +2554,34 @@
         <v>33</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I14" t="s">
         <v>23</v>
       </c>
       <c r="J14" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K14" t="s">
         <v>10</v>
       </c>
       <c r="L14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N14" t="s">
         <v>29</v>
       </c>
       <c r="O14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P14" t="s">
         <v>14</v>
       </c>
       <c r="Q14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R14" t="s">
         <v>6</v>
@@ -2609,31 +2593,31 @@
         <v>8</v>
       </c>
       <c r="U14" t="s">
+        <v>72</v>
+      </c>
+      <c r="V14" t="s">
+        <v>73</v>
+      </c>
+      <c r="W14" t="s">
+        <v>74</v>
+      </c>
+      <c r="X14" t="s">
         <v>75</v>
       </c>
-      <c r="V14" t="s">
+      <c r="Y14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z14" t="s">
         <v>76</v>
       </c>
-      <c r="W14" t="s">
+      <c r="AA14" t="s">
         <v>77</v>
       </c>
-      <c r="X14" t="s">
+      <c r="AB14" t="s">
         <v>78</v>
       </c>
-      <c r="Y14" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>81</v>
-      </c>
       <c r="AC14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AD14" t="s">
         <v>37</v>
@@ -2642,25 +2626,25 @@
         <v>36</v>
       </c>
       <c r="AF14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG14" t="s">
         <v>9</v>
       </c>
       <c r="AH14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI14" t="s">
         <v>7</v>
       </c>
       <c r="AJ14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AK14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AL14" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AM14" t="s">
         <v>15</v>
@@ -2672,31 +2656,31 @@
         <v>17</v>
       </c>
       <c r="AP14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU14" t="s">
         <v>85</v>
       </c>
-      <c r="AQ14" t="s">
+      <c r="AV14" t="s">
         <v>86</v>
       </c>
-      <c r="AR14" t="s">
+      <c r="AW14" t="s">
         <v>87</v>
       </c>
-      <c r="AS14" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT14" t="s">
+      <c r="AX14" t="s">
         <v>59</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV14" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW14" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX14" t="s">
-        <v>62</v>
       </c>
       <c r="AY14" t="s">
         <v>43</v>
@@ -2705,45 +2689,45 @@
         <v>42</v>
       </c>
       <c r="BA14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="BB14" t="s">
         <v>18</v>
       </c>
       <c r="BC14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="BD14" t="s">
         <v>16</v>
       </c>
       <c r="BE14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="BF14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="BG14" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="BH14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="BI14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="BJ14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="BK14" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -2752,7 +2736,7 @@
         <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
@@ -2761,34 +2745,34 @@
         <v>33</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I15" t="s">
         <v>23</v>
       </c>
       <c r="J15" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K15" t="s">
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N15" t="s">
         <v>29</v>
       </c>
       <c r="O15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P15" t="s">
         <v>14</v>
       </c>
       <c r="Q15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R15" t="s">
         <v>6</v>
@@ -2800,31 +2784,31 @@
         <v>8</v>
       </c>
       <c r="U15" t="s">
+        <v>72</v>
+      </c>
+      <c r="V15" t="s">
+        <v>73</v>
+      </c>
+      <c r="W15" t="s">
+        <v>74</v>
+      </c>
+      <c r="X15" t="s">
         <v>75</v>
       </c>
-      <c r="V15" t="s">
+      <c r="Y15" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z15" t="s">
         <v>76</v>
       </c>
-      <c r="W15" t="s">
+      <c r="AA15" t="s">
         <v>77</v>
       </c>
-      <c r="X15" t="s">
+      <c r="AB15" t="s">
         <v>78</v>
       </c>
-      <c r="Y15" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA15" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>81</v>
-      </c>
       <c r="AC15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AD15" t="s">
         <v>37</v>
@@ -2833,25 +2817,25 @@
         <v>36</v>
       </c>
       <c r="AF15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG15" t="s">
         <v>9</v>
       </c>
       <c r="AH15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI15" t="s">
         <v>7</v>
       </c>
       <c r="AJ15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AK15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AL15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AM15" t="s">
         <v>15</v>
@@ -2863,31 +2847,31 @@
         <v>17</v>
       </c>
       <c r="AP15" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU15" t="s">
         <v>85</v>
       </c>
-      <c r="AQ15" t="s">
+      <c r="AV15" t="s">
         <v>86</v>
       </c>
-      <c r="AR15" t="s">
+      <c r="AW15" t="s">
         <v>87</v>
       </c>
-      <c r="AS15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT15" t="s">
+      <c r="AX15" t="s">
         <v>59</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW15" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX15" t="s">
-        <v>62</v>
       </c>
       <c r="AY15" t="s">
         <v>43</v>
@@ -2896,45 +2880,45 @@
         <v>42</v>
       </c>
       <c r="BA15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="BB15" t="s">
         <v>18</v>
       </c>
       <c r="BC15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="BD15" t="s">
         <v>16</v>
       </c>
       <c r="BE15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="BF15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="BG15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="BH15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="BI15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="BJ15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="BK15" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
@@ -2943,7 +2927,7 @@
         <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
         <v>3</v>
@@ -2952,34 +2936,34 @@
         <v>33</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I16" t="s">
         <v>23</v>
       </c>
       <c r="J16" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K16" t="s">
         <v>10</v>
       </c>
       <c r="L16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="M16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="N16" t="s">
         <v>29</v>
       </c>
       <c r="O16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="P16" t="s">
         <v>14</v>
       </c>
       <c r="Q16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="R16" t="s">
         <v>6</v>
@@ -2991,31 +2975,31 @@
         <v>8</v>
       </c>
       <c r="U16" t="s">
+        <v>72</v>
+      </c>
+      <c r="V16" t="s">
+        <v>73</v>
+      </c>
+      <c r="W16" t="s">
+        <v>74</v>
+      </c>
+      <c r="X16" t="s">
         <v>75</v>
       </c>
-      <c r="V16" t="s">
+      <c r="Y16" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z16" t="s">
         <v>76</v>
       </c>
-      <c r="W16" t="s">
+      <c r="AA16" t="s">
         <v>77</v>
       </c>
-      <c r="X16" t="s">
+      <c r="AB16" t="s">
         <v>78</v>
       </c>
-      <c r="Y16" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>81</v>
-      </c>
       <c r="AC16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="AD16" t="s">
         <v>37</v>
@@ -3024,25 +3008,25 @@
         <v>36</v>
       </c>
       <c r="AF16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="AG16" t="s">
         <v>9</v>
       </c>
       <c r="AH16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="AI16" t="s">
         <v>7</v>
       </c>
       <c r="AJ16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AK16" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AL16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="AM16" t="s">
         <v>15</v>
@@ -3054,31 +3038,31 @@
         <v>17</v>
       </c>
       <c r="AP16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ16" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AS16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU16" t="s">
         <v>85</v>
       </c>
-      <c r="AQ16" t="s">
+      <c r="AV16" t="s">
         <v>86</v>
       </c>
-      <c r="AR16" t="s">
+      <c r="AW16" t="s">
         <v>87</v>
       </c>
-      <c r="AS16" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT16" t="s">
+      <c r="AX16" t="s">
         <v>59</v>
-      </c>
-      <c r="AU16" t="s">
-        <v>89</v>
-      </c>
-      <c r="AV16" t="s">
-        <v>90</v>
-      </c>
-      <c r="AW16" t="s">
-        <v>91</v>
-      </c>
-      <c r="AX16" t="s">
-        <v>62</v>
       </c>
       <c r="AY16" t="s">
         <v>43</v>
@@ -3087,316 +3071,314 @@
         <v>42</v>
       </c>
       <c r="BA16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="BB16" t="s">
         <v>18</v>
       </c>
       <c r="BC16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="BD16" t="s">
         <v>16</v>
       </c>
       <c r="BE16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="BF16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="BG16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="BH16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="BI16" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="BJ16" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="BK16" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.3">
-      <c r="A17"/>
-    </row>
-    <row r="18" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I18" t="s">
         <v>23</v>
       </c>
       <c r="J18" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K18" t="s">
         <v>10</v>
       </c>
       <c r="L18" t="s">
+        <v>105</v>
+      </c>
+      <c r="M18" t="s">
+        <v>106</v>
+      </c>
+      <c r="N18" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" t="s">
+        <v>108</v>
+      </c>
+      <c r="P18" t="s">
         <v>109</v>
       </c>
-      <c r="M18" t="s">
+      <c r="Q18" t="s">
         <v>110</v>
       </c>
-      <c r="N18" t="s">
+      <c r="R18" t="s">
         <v>111</v>
       </c>
-      <c r="O18" t="s">
+      <c r="S18" t="s">
         <v>112</v>
       </c>
-      <c r="P18" t="s">
+      <c r="T18" t="s">
         <v>113</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="U18" t="s">
         <v>114</v>
       </c>
-      <c r="R18" t="s">
+      <c r="V18" t="s">
         <v>115</v>
       </c>
-      <c r="S18" t="s">
+      <c r="W18" t="s">
         <v>116</v>
       </c>
-      <c r="T18" t="s">
+      <c r="X18" t="s">
         <v>117</v>
       </c>
-      <c r="U18" t="s">
+      <c r="Y18" t="s">
         <v>118</v>
       </c>
-      <c r="V18" t="s">
+      <c r="Z18" t="s">
         <v>119</v>
       </c>
-      <c r="W18" t="s">
+      <c r="AA18" t="s">
         <v>120</v>
       </c>
-      <c r="X18" t="s">
+      <c r="AB18" t="s">
         <v>121</v>
       </c>
-      <c r="Y18" t="s">
+      <c r="AC18" t="s">
         <v>122</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AD18" t="s">
         <v>123</v>
       </c>
-      <c r="AA18" t="s">
+      <c r="AE18" t="s">
         <v>124</v>
       </c>
-      <c r="AB18" t="s">
+      <c r="AF18" t="s">
         <v>125</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="AG18" t="s">
         <v>126</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AH18" t="s">
         <v>127</v>
       </c>
-      <c r="AE18" t="s">
+      <c r="AI18" t="s">
         <v>128</v>
       </c>
-      <c r="AF18" t="s">
+      <c r="AJ18" t="s">
         <v>129</v>
       </c>
-      <c r="AG18" t="s">
+      <c r="AK18" t="s">
         <v>130</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AL18" t="s">
         <v>131</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AM18" t="s">
         <v>132</v>
       </c>
-      <c r="AJ18" t="s">
+      <c r="AN18" t="s">
         <v>133</v>
       </c>
-      <c r="AK18" t="s">
+      <c r="AO18" t="s">
         <v>134</v>
       </c>
-      <c r="AL18" t="s">
+      <c r="AP18" t="s">
         <v>135</v>
       </c>
-      <c r="AM18" t="s">
+      <c r="AQ18" t="s">
         <v>136</v>
       </c>
-      <c r="AN18" t="s">
+      <c r="AR18" t="s">
         <v>137</v>
       </c>
-      <c r="AO18" t="s">
+      <c r="AS18" t="s">
         <v>138</v>
       </c>
-      <c r="AP18" t="s">
+      <c r="AT18" t="s">
         <v>139</v>
       </c>
-      <c r="AQ18" t="s">
+      <c r="AU18" t="s">
         <v>140</v>
       </c>
-      <c r="AR18" t="s">
+      <c r="AV18" t="s">
         <v>141</v>
       </c>
-      <c r="AS18" t="s">
+      <c r="AW18" t="s">
         <v>142</v>
       </c>
-      <c r="AT18" t="s">
+      <c r="AX18" t="s">
         <v>143</v>
       </c>
-      <c r="AU18" t="s">
+      <c r="AY18" t="s">
         <v>144</v>
       </c>
-      <c r="AV18" t="s">
+      <c r="AZ18" t="s">
         <v>145</v>
       </c>
-      <c r="AW18" t="s">
+      <c r="BA18" t="s">
         <v>146</v>
       </c>
-      <c r="AX18" t="s">
+      <c r="BB18" t="s">
         <v>147</v>
       </c>
-      <c r="AY18" t="s">
+      <c r="BC18" t="s">
         <v>148</v>
       </c>
-      <c r="AZ18" t="s">
+      <c r="BD18" t="s">
         <v>149</v>
       </c>
-      <c r="BA18" t="s">
+      <c r="BE18" t="s">
         <v>150</v>
       </c>
-      <c r="BB18" t="s">
+      <c r="BF18" t="s">
         <v>151</v>
       </c>
-      <c r="BC18" t="s">
+      <c r="BG18" t="s">
         <v>152</v>
       </c>
-      <c r="BD18" t="s">
+      <c r="BH18" t="s">
         <v>153</v>
       </c>
-      <c r="BE18" t="s">
+      <c r="BI18" t="s">
         <v>154</v>
       </c>
-      <c r="BF18" t="s">
+      <c r="BJ18" t="s">
         <v>155</v>
       </c>
-      <c r="BG18" t="s">
+      <c r="BK18" t="s">
         <v>156</v>
       </c>
-      <c r="BH18" t="s">
-        <v>157</v>
-      </c>
-      <c r="BI18" t="s">
-        <v>158</v>
-      </c>
-      <c r="BJ18" t="s">
-        <v>159</v>
-      </c>
-      <c r="BK18" t="s">
-        <v>160</v>
-      </c>
     </row>
-    <row r="19" spans="1:63" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="6"/>
+    <row r="19" spans="1:63" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
     </row>
-    <row r="20" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
     </row>
-    <row r="21" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
     </row>
-    <row r="22" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
     </row>
-    <row r="23" spans="1:63" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="9"/>
-      <c r="AE23" s="9"/>
-      <c r="AF23" s="9"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
-      <c r="AI23" s="9"/>
-      <c r="AJ23" s="9"/>
-      <c r="AK23" s="9"/>
-      <c r="AL23" s="9"/>
-      <c r="AM23" s="9"/>
-      <c r="AN23" s="9"/>
-      <c r="AO23" s="9"/>
-      <c r="AP23" s="9"/>
-      <c r="AQ23" s="9"/>
-      <c r="AR23" s="9"/>
-      <c r="AS23" s="9"/>
-      <c r="AT23" s="9"/>
-      <c r="AU23" s="9"/>
-      <c r="AV23" s="9"/>
-      <c r="AW23" s="9"/>
-      <c r="AX23" s="9"/>
-      <c r="AY23" s="9"/>
-      <c r="AZ23" s="9"/>
-      <c r="BA23" s="9"/>
-      <c r="BB23" s="9"/>
-      <c r="BC23" s="9"/>
-      <c r="BD23" s="9"/>
-      <c r="BE23" s="9"/>
-      <c r="BF23" s="9"/>
-      <c r="BG23" s="9"/>
-      <c r="BH23" s="9"/>
-      <c r="BI23" s="9"/>
-      <c r="BJ23" s="9"/>
+    <row r="23" spans="1:63" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10"/>
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="10"/>
+      <c r="AF23" s="10"/>
+      <c r="AG23" s="10"/>
+      <c r="AH23" s="10"/>
+      <c r="AI23" s="10"/>
+      <c r="AJ23" s="10"/>
+      <c r="AK23" s="10"/>
+      <c r="AL23" s="10"/>
+      <c r="AM23" s="10"/>
+      <c r="AN23" s="10"/>
+      <c r="AO23" s="10"/>
+      <c r="AP23" s="10"/>
+      <c r="AQ23" s="10"/>
+      <c r="AR23" s="10"/>
+      <c r="AS23" s="10"/>
+      <c r="AT23" s="10"/>
+      <c r="AU23" s="10"/>
+      <c r="AV23" s="10"/>
+      <c r="AW23" s="10"/>
+      <c r="AX23" s="10"/>
+      <c r="AY23" s="10"/>
+      <c r="AZ23" s="10"/>
+      <c r="BA23" s="10"/>
+      <c r="BB23" s="10"/>
+      <c r="BC23" s="10"/>
+      <c r="BD23" s="10"/>
+      <c r="BE23" s="10"/>
+      <c r="BF23" s="10"/>
+      <c r="BG23" s="10"/>
+      <c r="BH23" s="10"/>
+      <c r="BI23" s="10"/>
+      <c r="BJ23" s="10"/>
     </row>
-    <row r="24" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
     </row>
-    <row r="25" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:63" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
     </row>
   </sheetData>

</xml_diff>